<commit_message>
Add parser for capability support matrix with the same index architecture as the textbook
</commit_message>
<xml_diff>
--- a/graphdb-parser/sources/Data/Capability_Support_Matrix_V1_As-is.xlsx
+++ b/graphdb-parser/sources/Data/Capability_Support_Matrix_V1_As-is.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/U777053/Documents/Uni/FraUAS/Masterarbeit/prototype/graphdb-parser/sources/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DFBFB34-F77D-6046-87A7-1CA74DB03239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE30C407-E42A-9642-B28A-5A7BDA80F266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="500" windowWidth="38080" windowHeight="16140" xr2:uid="{38AA382D-BE5F-C04E-9040-C5DF4C9F6C44}"/>
+    <workbookView xWindow="2240" yWindow="880" windowWidth="38080" windowHeight="16140" xr2:uid="{38AA382D-BE5F-C04E-9040-C5DF4C9F6C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Capability Support Matrix" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>API Gateway</t>
   </si>
   <si>
-    <t>StatMan+</t>
-  </si>
-  <si>
     <t>StatMan</t>
   </si>
   <si>
@@ -516,6 +513,9 @@
   </si>
   <si>
     <t>Employee Performance Management</t>
+  </si>
+  <si>
+    <t>StatManPlus</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -675,15 +675,14 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
     <dxf>
@@ -814,10 +813,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{655ECD8C-4A40-0741-B359-60A99CD7CC71}" name="Tabelle3" displayName="Tabelle3" ref="A1:AJ123" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A1:AJ123" xr:uid="{655ECD8C-4A40-0741-B359-60A99CD7CC71}"/>
@@ -830,7 +825,7 @@
     <tableColumn id="7" xr3:uid="{4F724543-2899-BE45-ADEE-48CB33389626}" name="WiseGuy" dataDxfId="10"/>
     <tableColumn id="8" xr3:uid="{2154F65C-7149-3E48-BD42-1950B05C62EF}" name="CnCustoms" dataDxfId="9"/>
     <tableColumn id="9" xr3:uid="{240AFEF0-9586-A244-969D-E2D6226B4C77}" name="API Gateway"/>
-    <tableColumn id="10" xr3:uid="{8CF74D4F-7A01-1349-A337-7BA1D1E1298C}" name="StatMan+"/>
+    <tableColumn id="10" xr3:uid="{8CF74D4F-7A01-1349-A337-7BA1D1E1298C}" name="StatManPlus"/>
     <tableColumn id="11" xr3:uid="{6D297E20-43F2-1548-9EC3-9E7F72274EEE}" name="StatMan" dataDxfId="8"/>
     <tableColumn id="12" xr3:uid="{80545E17-FC90-7240-9B38-7032B054C77C}" name="LMD System" dataDxfId="7"/>
     <tableColumn id="13" xr3:uid="{B747AEA1-2CD8-D949-919C-F27519A2D4F1}" name="TrackDB"/>
@@ -1184,7 +1179,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A63" sqref="A63"/>
+      <selection pane="topRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1239,93 +1234,93 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="Y1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AB1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AD1" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AF1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AG1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AH1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="AE1" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="AF1" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="AG1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="AJ1" s="8" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="22" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3"/>
       <c r="D2"/>
@@ -1344,7 +1339,7 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="3"/>
       <c r="D3"/>
@@ -1355,7 +1350,7 @@
       <c r="L3"/>
       <c r="O3" s="3"/>
       <c r="S3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V3" s="3"/>
       <c r="W3"/>
@@ -1365,11 +1360,11 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3"/>
       <c r="G4" s="3"/>
@@ -1378,7 +1373,7 @@
       <c r="L4"/>
       <c r="O4" s="3"/>
       <c r="S4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V4" s="3"/>
       <c r="W4"/>
@@ -1386,19 +1381,19 @@
       <c r="Y4"/>
       <c r="AB4" s="3"/>
       <c r="AD4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3"/>
       <c r="G5" s="3"/>
@@ -1407,7 +1402,7 @@
       <c r="L5"/>
       <c r="O5" s="3"/>
       <c r="S5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V5" s="3"/>
       <c r="W5"/>
@@ -1415,17 +1410,17 @@
       <c r="Y5"/>
       <c r="AB5" s="3"/>
       <c r="AD5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:36" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>35</v>
+      <c r="A6" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -1434,22 +1429,22 @@
       <c r="K6" s="13"/>
       <c r="O6" s="13"/>
       <c r="S6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V6" s="13"/>
       <c r="X6" s="13"/>
       <c r="AA6" s="13"/>
       <c r="AB6" s="13"/>
       <c r="AC6" s="13"/>
-      <c r="AH6" s="17"/>
+      <c r="AH6" s="16"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="3"/>
       <c r="G7" s="3"/>
@@ -1464,12 +1459,12 @@
       <c r="Y7"/>
       <c r="AB7" s="3"/>
       <c r="AD7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3"/>
       <c r="D8"/>
@@ -1480,7 +1475,7 @@
       <c r="L8"/>
       <c r="O8" s="3"/>
       <c r="S8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V8" s="3"/>
       <c r="W8"/>
@@ -1488,12 +1483,12 @@
       <c r="Y8"/>
       <c r="AB8" s="3"/>
       <c r="AD8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>38</v>
+      <c r="A9" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="B9" s="4"/>
       <c r="D9"/>
@@ -1504,7 +1499,7 @@
       <c r="L9"/>
       <c r="O9" s="3"/>
       <c r="S9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V9" s="3"/>
       <c r="W9"/>
@@ -1512,12 +1507,12 @@
       <c r="Y9"/>
       <c r="AB9" s="3"/>
       <c r="AD9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4"/>
       <c r="D10"/>
@@ -1536,7 +1531,7 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3"/>
       <c r="D11"/>
@@ -1553,15 +1548,15 @@
       <c r="Y11"/>
       <c r="AB11" s="3"/>
       <c r="AD11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3"/>
       <c r="D12"/>
@@ -1578,12 +1573,12 @@
       <c r="Y12"/>
       <c r="AB12" s="3"/>
       <c r="AH12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3"/>
       <c r="D13"/>
@@ -1600,12 +1595,12 @@
       <c r="Y13"/>
       <c r="AB13" s="3"/>
       <c r="AH13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3"/>
       <c r="D14"/>
@@ -1622,12 +1617,12 @@
       <c r="Y14"/>
       <c r="AB14" s="3"/>
       <c r="AH14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3"/>
       <c r="D15"/>
@@ -1644,12 +1639,12 @@
       <c r="Y15"/>
       <c r="AB15" s="3"/>
       <c r="AH15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3"/>
       <c r="D16"/>
@@ -1668,7 +1663,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3"/>
       <c r="D17"/>
@@ -1685,15 +1680,15 @@
       <c r="Y17"/>
       <c r="AB17" s="3"/>
       <c r="AE17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3"/>
       <c r="D18"/>
@@ -1710,12 +1705,12 @@
       <c r="Y18"/>
       <c r="AB18" s="3"/>
       <c r="AH18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3"/>
       <c r="D19"/>
@@ -1726,10 +1721,10 @@
       <c r="L19"/>
       <c r="O19" s="3"/>
       <c r="S19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V19" s="3"/>
       <c r="W19"/>
@@ -1737,12 +1732,12 @@
       <c r="Y19"/>
       <c r="AB19" s="3"/>
       <c r="AH19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="3"/>
       <c r="D20"/>
@@ -1759,12 +1754,12 @@
       <c r="Y20"/>
       <c r="AB20" s="3"/>
       <c r="AH20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3"/>
       <c r="D21"/>
@@ -1781,12 +1776,12 @@
       <c r="Y21"/>
       <c r="AB21" s="3"/>
       <c r="AH21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3"/>
       <c r="D22"/>
@@ -1805,11 +1800,11 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="3"/>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="3"/>
       <c r="G23" s="3"/>
@@ -1818,7 +1813,7 @@
       <c r="L23"/>
       <c r="O23" s="3"/>
       <c r="S23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V23" s="3"/>
       <c r="W23"/>
@@ -1826,21 +1821,21 @@
       <c r="Y23"/>
       <c r="AB23" s="3"/>
       <c r="AD23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="3"/>
       <c r="G24" s="3"/>
@@ -1849,7 +1844,7 @@
       <c r="L24"/>
       <c r="O24" s="3"/>
       <c r="S24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V24" s="3"/>
       <c r="W24"/>
@@ -1857,24 +1852,24 @@
       <c r="Y24"/>
       <c r="AB24" s="3"/>
       <c r="AD24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G25" s="3"/>
       <c r="J25" s="3"/>
@@ -1882,7 +1877,7 @@
       <c r="L25"/>
       <c r="O25" s="3"/>
       <c r="S25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V25" s="3"/>
       <c r="W25"/>
@@ -1890,16 +1885,16 @@
       <c r="Y25"/>
       <c r="AB25" s="3"/>
       <c r="AD25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3"/>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="3"/>
       <c r="G26" s="3"/>
@@ -1914,12 +1909,12 @@
       <c r="Y26"/>
       <c r="AB26" s="3"/>
       <c r="AD26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:34" ht="22" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="3"/>
       <c r="D27"/>
@@ -1938,7 +1933,7 @@
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="3"/>
       <c r="D28"/>
@@ -1957,7 +1952,7 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="3"/>
       <c r="D29"/>
@@ -1969,10 +1964,10 @@
       <c r="O29" s="3"/>
       <c r="S29"/>
       <c r="T29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V29" s="3"/>
       <c r="W29"/>
@@ -1982,7 +1977,7 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3"/>
       <c r="D30"/>
@@ -1994,7 +1989,7 @@
       <c r="O30" s="3"/>
       <c r="S30"/>
       <c r="T30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V30" s="3"/>
       <c r="W30"/>
@@ -2004,7 +1999,7 @@
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="3"/>
       <c r="D31"/>
@@ -2016,10 +2011,10 @@
       <c r="O31" s="3"/>
       <c r="S31"/>
       <c r="T31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V31" s="3"/>
       <c r="W31"/>
@@ -2029,7 +2024,7 @@
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="3"/>
       <c r="D32"/>
@@ -2041,7 +2036,7 @@
       <c r="O32" s="3"/>
       <c r="S32"/>
       <c r="T32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V32" s="3"/>
       <c r="W32"/>
@@ -2051,7 +2046,7 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="3"/>
       <c r="D33"/>
@@ -2063,10 +2058,10 @@
       <c r="O33" s="3"/>
       <c r="S33"/>
       <c r="T33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V33" s="3"/>
       <c r="W33"/>
@@ -2076,7 +2071,7 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="3"/>
       <c r="D34"/>
@@ -2088,10 +2083,10 @@
       <c r="O34" s="3"/>
       <c r="S34"/>
       <c r="T34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V34" s="3"/>
       <c r="W34"/>
@@ -2101,7 +2096,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="3"/>
       <c r="D35"/>
@@ -2120,23 +2115,23 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="3"/>
       <c r="D36"/>
       <c r="E36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36"/>
       <c r="M36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O36" s="3"/>
       <c r="S36"/>
@@ -2148,23 +2143,23 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3"/>
       <c r="D37"/>
       <c r="E37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37"/>
       <c r="M37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O37" s="3"/>
       <c r="S37"/>
@@ -2176,7 +2171,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="3"/>
       <c r="D38"/>
@@ -2186,7 +2181,7 @@
       <c r="K38" s="3"/>
       <c r="L38"/>
       <c r="M38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O38" s="3"/>
       <c r="S38"/>
@@ -2198,19 +2193,19 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="3"/>
       <c r="D39"/>
       <c r="E39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O39" s="3"/>
       <c r="S39"/>
@@ -2222,7 +2217,7 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="3"/>
       <c r="D40"/>
@@ -2241,16 +2236,16 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" s="3"/>
       <c r="D41"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2263,24 +2258,24 @@
       <c r="Y41"/>
       <c r="AB41" s="3"/>
       <c r="AE41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" s="3"/>
       <c r="D42"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O42" s="3"/>
       <c r="S42"/>
@@ -2290,24 +2285,24 @@
       <c r="Y42"/>
       <c r="AB42" s="3"/>
       <c r="AE42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" s="3"/>
       <c r="D43"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O43" s="3"/>
       <c r="S43"/>
@@ -2317,12 +2312,12 @@
       <c r="Y43"/>
       <c r="AB43" s="3"/>
       <c r="AE43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B44" s="3"/>
       <c r="D44"/>
@@ -2334,7 +2329,7 @@
       <c r="O44" s="3"/>
       <c r="S44"/>
       <c r="T44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V44" s="3"/>
       <c r="W44"/>
@@ -2342,18 +2337,18 @@
       <c r="Y44"/>
       <c r="AB44" s="3"/>
       <c r="AE44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B45" s="3"/>
       <c r="D45"/>
       <c r="E45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -2366,12 +2361,12 @@
       <c r="Y45"/>
       <c r="AB45" s="3"/>
       <c r="AE45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46" s="3"/>
       <c r="D46"/>
@@ -2390,7 +2385,7 @@
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" s="3"/>
       <c r="D47"/>
@@ -2403,7 +2398,7 @@
       <c r="S47"/>
       <c r="V47" s="3"/>
       <c r="W47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X47" s="3"/>
       <c r="Y47"/>
@@ -2411,16 +2406,16 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E48" s="3"/>
       <c r="G48" s="3"/>
@@ -2431,7 +2426,7 @@
       <c r="S48"/>
       <c r="V48" s="3"/>
       <c r="W48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X48" s="3"/>
       <c r="Y48"/>
@@ -2439,13 +2434,13 @@
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D49"/>
       <c r="E49" s="3"/>
@@ -2457,7 +2452,7 @@
       <c r="S49"/>
       <c r="V49" s="3"/>
       <c r="W49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X49" s="3"/>
       <c r="Y49"/>
@@ -2465,7 +2460,7 @@
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B50" s="3"/>
       <c r="D50"/>
@@ -2478,7 +2473,7 @@
       <c r="S50"/>
       <c r="V50" s="3"/>
       <c r="W50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X50" s="3"/>
       <c r="Y50"/>
@@ -2486,11 +2481,11 @@
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" s="3"/>
       <c r="D51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E51" s="3"/>
       <c r="G51" s="3"/>
@@ -2501,7 +2496,7 @@
       <c r="S51"/>
       <c r="V51" s="3"/>
       <c r="W51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X51" s="3"/>
       <c r="Y51"/>
@@ -2509,7 +2504,7 @@
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B52" s="3"/>
       <c r="D52"/>
@@ -2528,14 +2523,14 @@
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B53" s="3"/>
       <c r="D53"/>
       <c r="E53" s="3"/>
       <c r="G53" s="3"/>
       <c r="I53" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2550,19 +2545,19 @@
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B54" s="3"/>
       <c r="D54"/>
       <c r="E54" s="3"/>
       <c r="G54" s="3"/>
       <c r="I54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O54" s="3"/>
       <c r="S54"/>
@@ -2574,14 +2569,14 @@
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B55" s="3"/>
       <c r="D55"/>
       <c r="E55" s="3"/>
       <c r="G55" s="3"/>
       <c r="I55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -2596,21 +2591,21 @@
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B56" s="3"/>
       <c r="D56"/>
       <c r="E56" s="3"/>
       <c r="G56" s="3"/>
       <c r="I56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O56" s="3"/>
       <c r="S56"/>
@@ -2622,7 +2617,7 @@
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B57" s="3"/>
       <c r="D57"/>
@@ -2631,11 +2626,11 @@
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O57" s="3"/>
       <c r="P57" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S57"/>
       <c r="V57" s="3"/>
@@ -2646,7 +2641,7 @@
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B58" s="3"/>
       <c r="D58"/>
@@ -2665,7 +2660,7 @@
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" s="3"/>
       <c r="D59"/>
@@ -2676,7 +2671,7 @@
       <c r="L59"/>
       <c r="O59" s="3"/>
       <c r="P59" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S59"/>
       <c r="V59" s="3"/>
@@ -2687,23 +2682,23 @@
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B60" s="3"/>
       <c r="D60"/>
       <c r="E60" s="3"/>
       <c r="G60" s="3"/>
       <c r="I60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K60" s="3"/>
       <c r="L60"/>
       <c r="O60" s="3"/>
       <c r="P60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S60"/>
       <c r="V60" s="3"/>
@@ -2714,14 +2709,14 @@
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B61" s="3"/>
       <c r="D61"/>
       <c r="E61" s="3"/>
       <c r="G61" s="3"/>
       <c r="I61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -2736,14 +2731,14 @@
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B62" s="3"/>
       <c r="D62"/>
       <c r="E62" s="3"/>
       <c r="G62" s="3"/>
       <c r="I62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
@@ -2758,7 +2753,7 @@
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B63" s="3"/>
       <c r="D63"/>
@@ -2777,7 +2772,7 @@
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B64" s="3"/>
       <c r="D64"/>
@@ -2787,10 +2782,10 @@
       <c r="K64" s="3"/>
       <c r="L64"/>
       <c r="M64" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S64"/>
       <c r="V64" s="3"/>
@@ -2799,12 +2794,12 @@
       <c r="Y64"/>
       <c r="AB64" s="3"/>
       <c r="AE64" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B65" s="3"/>
       <c r="D65"/>
@@ -2814,10 +2809,10 @@
       <c r="K65" s="3"/>
       <c r="L65"/>
       <c r="M65" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S65"/>
       <c r="V65" s="3"/>
@@ -2826,12 +2821,12 @@
       <c r="Y65"/>
       <c r="AB65" s="3"/>
       <c r="AE65" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B66" s="3"/>
       <c r="D66"/>
@@ -2841,13 +2836,13 @@
       <c r="K66" s="3"/>
       <c r="L66"/>
       <c r="M66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S66"/>
       <c r="V66" s="3"/>
@@ -2856,12 +2851,12 @@
       <c r="Y66"/>
       <c r="AB66" s="3"/>
       <c r="AE66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B67" s="3"/>
       <c r="D67"/>
@@ -2871,10 +2866,10 @@
       <c r="K67" s="3"/>
       <c r="L67"/>
       <c r="M67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S67"/>
       <c r="V67" s="3"/>
@@ -2883,12 +2878,12 @@
       <c r="Y67"/>
       <c r="AB67" s="3"/>
       <c r="AE67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B68" s="3"/>
       <c r="D68"/>
@@ -2898,13 +2893,13 @@
       <c r="K68" s="3"/>
       <c r="L68"/>
       <c r="M68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S68"/>
       <c r="V68" s="3"/>
@@ -2913,12 +2908,12 @@
       <c r="Y68"/>
       <c r="AB68" s="3"/>
       <c r="AE68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B69" s="3"/>
       <c r="D69"/>
@@ -2935,12 +2930,12 @@
       <c r="Y69"/>
       <c r="AB69" s="3"/>
       <c r="AF69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B70" s="3"/>
       <c r="D70"/>
@@ -2957,12 +2952,12 @@
       <c r="Y70"/>
       <c r="AB70" s="3"/>
       <c r="AF70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B71" s="3"/>
       <c r="D71"/>
@@ -2979,12 +2974,12 @@
       <c r="Y71"/>
       <c r="AB71" s="3"/>
       <c r="AF71" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B72" s="3"/>
       <c r="D72"/>
@@ -3001,12 +2996,12 @@
       <c r="Y72"/>
       <c r="AB72" s="3"/>
       <c r="AF72" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B73" s="3"/>
       <c r="D73"/>
@@ -3023,12 +3018,12 @@
       <c r="Y73"/>
       <c r="AB73" s="3"/>
       <c r="AF73" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B74" s="3"/>
       <c r="D74"/>
@@ -3045,12 +3040,12 @@
       <c r="Y74"/>
       <c r="AB74" s="3"/>
       <c r="AF74" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="75" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B75" s="3"/>
       <c r="D75"/>
@@ -3069,11 +3064,11 @@
     </row>
     <row r="76" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B76" s="3"/>
       <c r="D76" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E76" s="3"/>
       <c r="G76" s="3"/>
@@ -3090,11 +3085,11 @@
     </row>
     <row r="77" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B77" s="3"/>
       <c r="D77" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E77" s="3"/>
       <c r="G77" s="3"/>
@@ -3110,8 +3105,8 @@
       <c r="AB77" s="3"/>
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A78" s="16" t="s">
-        <v>108</v>
+      <c r="A78" s="15" t="s">
+        <v>107</v>
       </c>
       <c r="B78" s="3"/>
       <c r="D78"/>
@@ -3128,12 +3123,12 @@
       <c r="Y78"/>
       <c r="AB78" s="3"/>
       <c r="AF78" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B79" s="3"/>
       <c r="D79"/>
@@ -3152,7 +3147,7 @@
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B80" s="3"/>
       <c r="D80"/>
@@ -3162,7 +3157,7 @@
       <c r="K80" s="3"/>
       <c r="L80"/>
       <c r="N80" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O80" s="3"/>
       <c r="S80"/>
@@ -3174,7 +3169,7 @@
     </row>
     <row r="81" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B81" s="3"/>
       <c r="D81"/>
@@ -3184,7 +3179,7 @@
       <c r="K81" s="3"/>
       <c r="L81"/>
       <c r="N81" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O81" s="3"/>
       <c r="S81"/>
@@ -3196,7 +3191,7 @@
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B82" s="3"/>
       <c r="D82"/>
@@ -3206,7 +3201,7 @@
       <c r="K82" s="3"/>
       <c r="L82"/>
       <c r="N82" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O82" s="3"/>
       <c r="S82"/>
@@ -3218,7 +3213,7 @@
     </row>
     <row r="83" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B83" s="3"/>
       <c r="D83"/>
@@ -3228,10 +3223,10 @@
       <c r="K83" s="3"/>
       <c r="L83"/>
       <c r="M83" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N83" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O83" s="3"/>
       <c r="S83"/>
@@ -3243,7 +3238,7 @@
     </row>
     <row r="84" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B84" s="3"/>
       <c r="D84"/>
@@ -3262,7 +3257,7 @@
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B85" s="3"/>
       <c r="D85"/>
@@ -3275,18 +3270,18 @@
       <c r="S85"/>
       <c r="V85" s="3"/>
       <c r="W85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X85" s="3"/>
       <c r="Y85"/>
       <c r="AB85" s="3"/>
       <c r="AF85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B86" s="3"/>
       <c r="D86"/>
@@ -3299,18 +3294,18 @@
       <c r="S86"/>
       <c r="V86" s="3"/>
       <c r="W86" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X86" s="3"/>
       <c r="Y86"/>
       <c r="AB86" s="3"/>
       <c r="AF86" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B87" s="3"/>
       <c r="D87"/>
@@ -3327,12 +3322,12 @@
       <c r="Y87"/>
       <c r="AB87" s="3"/>
       <c r="AF87" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B88" s="3"/>
       <c r="D88"/>
@@ -3345,18 +3340,18 @@
       <c r="S88"/>
       <c r="V88" s="3"/>
       <c r="W88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X88" s="3"/>
       <c r="Y88"/>
       <c r="AB88" s="3"/>
       <c r="AF88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B89" s="3"/>
       <c r="D89"/>
@@ -3369,18 +3364,18 @@
       <c r="S89"/>
       <c r="V89" s="3"/>
       <c r="W89" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X89" s="3"/>
       <c r="Y89"/>
       <c r="AB89" s="3"/>
       <c r="AF89" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:36" ht="22" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B90" s="3"/>
       <c r="D90"/>
@@ -3399,7 +3394,7 @@
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B91" s="3"/>
       <c r="D91"/>
@@ -3418,7 +3413,7 @@
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B92" s="3"/>
       <c r="D92"/>
@@ -3435,15 +3430,15 @@
       <c r="Y92"/>
       <c r="AB92" s="3"/>
       <c r="AC92" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AJ92" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B93" s="3"/>
       <c r="D93"/>
@@ -3460,15 +3455,15 @@
       <c r="Y93"/>
       <c r="AB93" s="3"/>
       <c r="AC93" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AJ93" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B94" s="3"/>
       <c r="D94"/>
@@ -3485,15 +3480,15 @@
       <c r="Y94"/>
       <c r="AB94" s="3"/>
       <c r="AC94" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AJ94" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B95" s="3"/>
       <c r="D95"/>
@@ -3508,19 +3503,19 @@
       <c r="W95"/>
       <c r="X95" s="3"/>
       <c r="Y95" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB95" s="3"/>
       <c r="AC95" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AJ95" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B96" s="3"/>
       <c r="D96"/>
@@ -3537,15 +3532,15 @@
       <c r="Y96"/>
       <c r="AB96" s="3"/>
       <c r="AC96" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AJ96" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B97" s="3"/>
       <c r="D97"/>
@@ -3562,15 +3557,15 @@
       <c r="Y97"/>
       <c r="AB97" s="3"/>
       <c r="AC97" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AJ97" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B98" s="3"/>
       <c r="D98"/>
@@ -3587,15 +3582,15 @@
       <c r="Y98"/>
       <c r="AB98" s="3"/>
       <c r="AC98" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AJ98" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B99" s="3"/>
       <c r="D99"/>
@@ -3614,11 +3609,11 @@
     </row>
     <row r="100" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B100" s="3"/>
       <c r="D100" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E100" s="3"/>
       <c r="G100" s="3"/>
@@ -3629,7 +3624,7 @@
       <c r="S100"/>
       <c r="V100" s="3"/>
       <c r="W100" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X100" s="3"/>
       <c r="Y100"/>
@@ -3637,7 +3632,7 @@
     </row>
     <row r="101" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B101" s="3"/>
       <c r="D101"/>
@@ -3649,11 +3644,11 @@
       <c r="O101" s="3"/>
       <c r="S101"/>
       <c r="U101" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V101" s="3"/>
       <c r="W101" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X101" s="3"/>
       <c r="Y101"/>
@@ -3661,11 +3656,11 @@
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B102" s="3"/>
       <c r="D102" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E102" s="3"/>
       <c r="G102" s="3"/>
@@ -3676,7 +3671,7 @@
       <c r="S102"/>
       <c r="V102" s="3"/>
       <c r="W102" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X102" s="3"/>
       <c r="Y102"/>
@@ -3684,11 +3679,11 @@
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B103" s="3"/>
       <c r="D103" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E103" s="3"/>
       <c r="G103" s="3"/>
@@ -3699,7 +3694,7 @@
       <c r="S103"/>
       <c r="V103" s="3"/>
       <c r="W103" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X103" s="3"/>
       <c r="Y103"/>
@@ -3707,11 +3702,11 @@
     </row>
     <row r="104" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B104" s="3"/>
       <c r="D104" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E104" s="3"/>
       <c r="G104" s="3"/>
@@ -3722,7 +3717,7 @@
       <c r="S104"/>
       <c r="V104" s="3"/>
       <c r="W104" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X104" s="3"/>
       <c r="Y104"/>
@@ -3730,7 +3725,7 @@
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B105" s="3"/>
       <c r="D105"/>
@@ -3749,7 +3744,7 @@
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B106" s="3"/>
       <c r="D106"/>
@@ -3765,16 +3760,16 @@
       <c r="X106" s="3"/>
       <c r="Y106"/>
       <c r="AA106" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB106" s="3"/>
       <c r="AI106" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="107" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B107" s="3"/>
       <c r="D107"/>
@@ -3790,16 +3785,16 @@
       <c r="X107" s="3"/>
       <c r="Y107"/>
       <c r="AA107" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB107" s="3"/>
       <c r="AI107" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B108" s="3"/>
       <c r="D108"/>
@@ -3815,16 +3810,16 @@
       <c r="X108" s="3"/>
       <c r="Y108"/>
       <c r="AA108" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB108" s="3"/>
       <c r="AI108" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="109" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B109" s="3"/>
       <c r="D109"/>
@@ -3840,18 +3835,18 @@
       <c r="X109" s="3"/>
       <c r="Y109"/>
       <c r="AA109" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB109" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI109" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B110" s="3"/>
       <c r="D110"/>
@@ -3863,26 +3858,26 @@
       <c r="O110" s="3"/>
       <c r="S110"/>
       <c r="T110" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U110" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V110" s="3"/>
       <c r="W110"/>
       <c r="X110" s="3"/>
       <c r="Y110"/>
       <c r="AA110" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB110" s="3"/>
       <c r="AI110" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B111" s="3"/>
       <c r="D111"/>
@@ -3901,7 +3896,7 @@
     </row>
     <row r="112" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B112" s="3"/>
       <c r="D112"/>
@@ -3913,10 +3908,10 @@
       <c r="O112" s="3"/>
       <c r="S112"/>
       <c r="T112" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U112" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V112" s="3"/>
       <c r="W112"/>
@@ -3924,12 +3919,12 @@
       <c r="Y112"/>
       <c r="AB112" s="3"/>
       <c r="AH112" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="113" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B113" s="3"/>
       <c r="D113"/>
@@ -3940,13 +3935,13 @@
       <c r="L113"/>
       <c r="O113" s="3"/>
       <c r="R113" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S113" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T113" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V113" s="3"/>
       <c r="W113"/>
@@ -3954,15 +3949,15 @@
       <c r="Y113"/>
       <c r="AB113" s="3"/>
       <c r="AG113" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH113" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B114" s="3"/>
       <c r="D114"/>
@@ -3973,10 +3968,10 @@
       <c r="L114"/>
       <c r="O114" s="3"/>
       <c r="R114" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S114" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V114" s="3"/>
       <c r="W114"/>
@@ -3984,15 +3979,15 @@
       <c r="Y114"/>
       <c r="AB114" s="3"/>
       <c r="AD114" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH114" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="115" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B115" s="3"/>
       <c r="D115"/>
@@ -4003,10 +3998,10 @@
       <c r="L115"/>
       <c r="O115" s="3"/>
       <c r="R115" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S115" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V115" s="3"/>
       <c r="W115"/>
@@ -4014,15 +4009,15 @@
       <c r="Y115"/>
       <c r="AB115" s="3"/>
       <c r="AD115" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH115" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B116" s="3"/>
       <c r="D116"/>
@@ -4041,7 +4036,7 @@
     </row>
     <row r="117" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B117" s="3"/>
       <c r="D117"/>
@@ -4056,13 +4051,13 @@
       <c r="W117"/>
       <c r="X117" s="3"/>
       <c r="Y117" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB117" s="3"/>
     </row>
     <row r="118" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B118" s="3"/>
       <c r="D118"/>
@@ -4077,13 +4072,13 @@
       <c r="W118"/>
       <c r="X118" s="3"/>
       <c r="Y118" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB118" s="3"/>
     </row>
     <row r="119" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B119" s="3"/>
       <c r="D119"/>
@@ -4098,13 +4093,13 @@
       <c r="W119"/>
       <c r="X119" s="3"/>
       <c r="Y119" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB119" s="3"/>
     </row>
     <row r="120" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B120" s="3"/>
       <c r="D120"/>
@@ -4123,11 +4118,11 @@
     </row>
     <row r="121" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B121" s="3"/>
       <c r="D121" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E121" s="3"/>
       <c r="G121" s="3"/>
@@ -4138,7 +4133,7 @@
       <c r="S121"/>
       <c r="V121" s="3"/>
       <c r="W121" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X121" s="3"/>
       <c r="Y121"/>
@@ -4146,13 +4141,13 @@
     </row>
     <row r="122" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D122" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E122" s="3"/>
       <c r="G122" s="3"/>
@@ -4163,30 +4158,30 @@
       <c r="S122"/>
       <c r="V122" s="3"/>
       <c r="W122" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X122" s="3"/>
       <c r="Y122"/>
       <c r="Z122" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB122" s="3"/>
       <c r="AD122" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="123" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D123" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E123" s="3"/>
       <c r="G123" s="3"/>
@@ -4197,12 +4192,12 @@
       <c r="S123"/>
       <c r="V123" s="3"/>
       <c r="W123" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X123" s="3"/>
       <c r="Y123"/>
       <c r="Z123" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB123" s="3"/>
     </row>
@@ -4226,15 +4221,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3F6B6597720CC4C9E04F1341609415C" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="79d83348afde3d20d1dc47567965d351">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="27dda51f-07d3-489c-9f7c-f6e9375a2ada" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ad55fbc34f5ff11f1858669a401177fa" ns2:_="">
     <xsd:import namespace="27dda51f-07d3-489c-9f7c-f6e9375a2ada"/>
@@ -4372,6 +4358,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B11166A3-5273-4BA3-A360-25050A0BA377}">
   <ds:schemaRefs>
@@ -4389,14 +4384,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0831B22-82BC-446B-B1F4-B21093921163}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EAC1264-68A5-4FEF-A940-BE00C3E20E3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4412,4 +4399,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0831B22-82BC-446B-B1F4-B21093921163}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add parser for BOM
</commit_message>
<xml_diff>
--- a/graphdb-parser/sources/Data/Capability_Support_Matrix_V1_As-is.xlsx
+++ b/graphdb-parser/sources/Data/Capability_Support_Matrix_V1_As-is.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/U777053/Documents/Uni/FraUAS/Masterarbeit/prototype/graphdb-parser/sources/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE30C407-E42A-9642-B28A-5A7BDA80F266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1C8B2F-33AD-3547-9C79-7AD43C097DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="880" windowWidth="38080" windowHeight="16140" xr2:uid="{38AA382D-BE5F-C04E-9040-C5DF4C9F6C44}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="41120" windowHeight="25720" xr2:uid="{38AA382D-BE5F-C04E-9040-C5DF4C9F6C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Capability Support Matrix" sheetId="1" r:id="rId1"/>
@@ -1177,9 +1177,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997DA59A-8CDF-8C46-A0CD-240605B2CD14}">
   <dimension ref="A1:AJ123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H10" sqref="H10"/>
+      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4215,9 +4215,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4359,26 +4362,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B11166A3-5273-4BA3-A360-25050A0BA377}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0831B22-82BC-446B-B1F4-B21093921163}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="27dda51f-07d3-489c-9f7c-f6e9375a2ada"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4402,9 +4394,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0831B22-82BC-446B-B1F4-B21093921163}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B11166A3-5273-4BA3-A360-25050A0BA377}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="27dda51f-07d3-489c-9f7c-f6e9375a2ada"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add BOM and cross application data flow
</commit_message>
<xml_diff>
--- a/graphdb-parser/sources/Data/Capability_Support_Matrix_V1_As-is.xlsx
+++ b/graphdb-parser/sources/Data/Capability_Support_Matrix_V1_As-is.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/U777053/Documents/Uni/FraUAS/Masterarbeit/prototype/graphdb-parser/sources/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1C8B2F-33AD-3547-9C79-7AD43C097DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEB52A6-4C9E-B449-9BAC-6C29F34ACD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="41120" windowHeight="25720" xr2:uid="{38AA382D-BE5F-C04E-9040-C5DF4C9F6C44}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{38AA382D-BE5F-C04E-9040-C5DF4C9F6C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Capability Support Matrix" sheetId="1" r:id="rId1"/>
@@ -1179,7 +1179,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="topRight" activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4215,12 +4215,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4362,15 +4359,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0831B22-82BC-446B-B1F4-B21093921163}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B11166A3-5273-4BA3-A360-25050A0BA377}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="27dda51f-07d3-489c-9f7c-f6e9375a2ada"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4394,17 +4402,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B11166A3-5273-4BA3-A360-25050A0BA377}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0831B22-82BC-446B-B1F4-B21093921163}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="27dda51f-07d3-489c-9f7c-f6e9375a2ada"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>